<commit_message>
fitted report numbers data with ARIMA and inverse proportional curves
</commit_message>
<xml_diff>
--- a/src/dataset/wordle_data.xlsx
+++ b/src/dataset/wordle_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\03 - NYU Shanghai\8_Spring 2023\_MCM'23\MCM-23_2316597\src\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29522B2E-DFF1-48C7-8A90-511F4045F923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329CFEAD-BE9E-4ECD-B626-2E53D6408069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE11D8C7-548A-6E47-9F96-66C18673C8FF}"/>
   </bookViews>
@@ -1519,11 +1519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989317FD-0C58-6349-9F4F-FA56E36DDA65}">
-  <dimension ref="A1:L480"/>
+  <dimension ref="A1:O480"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A266" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G286" sqref="G286"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1541,7 +1541,7 @@
     <col min="13" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>356</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44926</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44925</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44924</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44923</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44922</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44921</v>
       </c>
@@ -1806,8 +1806,15 @@
       <c r="L7" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N7" s="3">
+        <v>44986</v>
+      </c>
+      <c r="O7" s="1">
+        <f>N7-A360</f>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>44920</v>
       </c>
@@ -1845,7 +1852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>44919</v>
       </c>
@@ -1883,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>44918</v>
       </c>
@@ -1921,7 +1928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>44917</v>
       </c>
@@ -1959,7 +1966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>44916</v>
       </c>
@@ -1997,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>44915</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>44914</v>
       </c>
@@ -2073,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>44913</v>
       </c>
@@ -2111,7 +2118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>44912</v>
       </c>

</xml_diff>

<commit_message>
updated curve fitting for question 1, please ignore report_num.ipynb for now
</commit_message>
<xml_diff>
--- a/src/dataset/wordle_data.xlsx
+++ b/src/dataset/wordle_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\03 - NYU Shanghai\8_Spring 2023\_MCM'23\MCM-23_2316597\src\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329CFEAD-BE9E-4ECD-B626-2E53D6408069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22047B2C-343A-4158-932C-06051750A6A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE11D8C7-548A-6E47-9F96-66C18673C8FF}"/>
   </bookViews>
@@ -1523,7 +1523,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
q1 done, moved correlation test to q2
</commit_message>
<xml_diff>
--- a/src/dataset/wordle_data.xlsx
+++ b/src/dataset/wordle_data.xlsx
@@ -1111,7 +1111,7 @@
     <t>abbey</t>
   </si>
   <si>
-    <t xml:space="preserve">favor </t>
+    <t>favor</t>
   </si>
   <si>
     <t>drink</t>
@@ -1134,7 +1134,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1145,6 +1145,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1193,8 +1199,8 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>

</xml_diff>

<commit_message>
final modifications before end of contest
</commit_message>
<xml_diff>
--- a/src/dataset/wordle_data.xlsx
+++ b/src/dataset/wordle_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\03 - NYU Shanghai\8_Spring 2023\_MCM'23\MCM-23_2316597\src\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A97CC3-C972-4A65-812D-7C54A94C7E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8129A28A-D2BD-49A3-97B0-D887933CD506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1524,7 +1524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1619,10 +1619,6 @@
       <c r="L2" s="2">
         <v>2</v>
       </c>
-      <c r="M2">
-        <f>1*F2+2*G2+3*H2+4*I2+5*J2+6*K2+7*L2</f>
-        <v>434</v>
-      </c>
     </row>
     <row r="3" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">

</xml_diff>